<commit_message>
resuelto frecuencias verticales y horizontales
</commit_message>
<xml_diff>
--- a/excel/exprebus-38-sabados-ns.xlsx
+++ b/excel/exprebus-38-sabados-ns.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRACTICAS_WEB\JAVASCRIPT\horabondi-algoritmo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRACTICAS_WEB\JAVASCRIPT\horabondi-algoritmo\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B929CD11-015A-4F10-A8C8-B14C7F9ACF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7100090C-C48E-4FE8-B131-F10BE0A1BD43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="11-12-2022" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="85">
   <si>
     <t>tucuman</t>
   </si>
@@ -247,6 +247,39 @@
   </si>
   <si>
     <t>[7,8,9]</t>
+  </si>
+  <si>
+    <t>RESULTADO FRECUENCIA VERTICAL CON PIVOTE POS 3, LONG 10</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>T-stamp</t>
+  </si>
+  <si>
+    <t>T-diff</t>
+  </si>
+  <si>
+    <t>30 min</t>
+  </si>
+  <si>
+    <t>Min =&gt; TS</t>
+  </si>
+  <si>
+    <t>60 min</t>
+  </si>
+  <si>
+    <t>40 min</t>
+  </si>
+  <si>
+    <t>50 min</t>
+  </si>
+  <si>
+    <t>12h20min</t>
+  </si>
+  <si>
+    <t>calcula el anterior y posterior, en el caso del final, no deberiamos tomar dicho valor</t>
   </si>
 </sst>
 </file>
@@ -740,10 +773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:J21"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1336,9 +1369,169 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="20" t="s">
         <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="6">
+        <v>0.28472222222222221</v>
+      </c>
+      <c r="C37" s="6">
+        <v>0.30555555555555552</v>
+      </c>
+      <c r="D37" s="6">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="E37" s="6">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="F37" s="6">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="G37" s="6">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="H37" s="6">
+        <v>0.4375</v>
+      </c>
+      <c r="I37" s="6">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="J37" s="6">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="K37" s="6">
+        <v>0.51388888888888895</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38">
+        <v>35400000</v>
+      </c>
+      <c r="C38">
+        <v>37200000</v>
+      </c>
+      <c r="D38">
+        <v>39000000</v>
+      </c>
+      <c r="E38">
+        <v>40800000</v>
+      </c>
+      <c r="F38">
+        <v>44400000</v>
+      </c>
+      <c r="G38">
+        <v>46200000</v>
+      </c>
+      <c r="H38">
+        <v>48600000</v>
+      </c>
+      <c r="I38">
+        <v>51600000</v>
+      </c>
+      <c r="J38">
+        <v>53400000</v>
+      </c>
+      <c r="K38">
+        <v>55200000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39">
+        <v>1800000</v>
+      </c>
+      <c r="C39">
+        <v>1800000</v>
+      </c>
+      <c r="D39">
+        <v>1800000</v>
+      </c>
+      <c r="E39">
+        <v>3600000</v>
+      </c>
+      <c r="F39">
+        <v>1800000</v>
+      </c>
+      <c r="G39">
+        <v>2400000</v>
+      </c>
+      <c r="H39">
+        <v>3000000</v>
+      </c>
+      <c r="I39">
+        <v>1800000</v>
+      </c>
+      <c r="J39">
+        <v>1800000</v>
+      </c>
+      <c r="K39">
+        <v>55200000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="24" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41">
+        <v>1800000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42">
+        <v>3600000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43">
+        <v>2400000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44">
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45">
+        <v>55200000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregada primera solucion, arreglo de frecuencias verticales
</commit_message>
<xml_diff>
--- a/excel/exprebus-38-sabados-ns.xlsx
+++ b/excel/exprebus-38-sabados-ns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRACTICAS_WEB\JAVASCRIPT\horabondi-algoritmo\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7100090C-C48E-4FE8-B131-F10BE0A1BD43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9B34E1-721A-4D4C-91BF-02B505522FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24255" yWindow="990" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="11-12-2022" sheetId="1" r:id="rId1"/>
@@ -775,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>